<commit_message>
dev1 changed test0.xlsx 2
</commit_message>
<xml_diff>
--- a/src/main/resources/test0.xlsx
+++ b/src/main/resources/test0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjectsD\TraningGit3\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CCE038-C3F5-48ED-B0B8-794386C375DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68D3E09-9BEF-48B1-9751-449598A1EED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,11 +353,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>